<commit_message>
updates to score_task, misc cleanup
</commit_message>
<xml_diff>
--- a/resources/whyhowlocalizer_iteminfo.xlsx
+++ b/resources/whyhowlocalizer_iteminfo.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-30460" yWindow="2900" windowWidth="25600" windowHeight="15080"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="25600" windowHeight="28260"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="blockwise" sheetId="2" r:id="rId1"/>
+    <sheet name="trialwise" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="109">
   <si>
     <t>Question Cue</t>
   </si>
@@ -328,13 +329,31 @@
   </si>
   <si>
     <t>both hands?</t>
+  </si>
+  <si>
+    <t>Emotion</t>
+  </si>
+  <si>
+    <t>Why</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>How</t>
+  </si>
+  <si>
+    <t>Stimulus</t>
+  </si>
+  <si>
+    <t>Question</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -347,13 +366,52 @@
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -365,10 +423,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -379,8 +441,27 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -710,10 +791,274 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="35.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G129" sqref="F2:G129"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -3697,6 +4042,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>